<commit_message>
Lesson 17 page object
</commit_message>
<xml_diff>
--- a/test data/Merchants data.xlsx
+++ b/test data/Merchants data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Java\TS_Maven\test data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telesens\SKMaven\test data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6561F220-A51E-4008-8CAD-AB8A5B36026E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B78580F-62BA-4CE4-A29E-8383100D8BE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C0DCDE7E-FD22-412E-8C09-E69394502170}"/>
+    <workbookView xWindow="2304" yWindow="2004" windowWidth="20148" windowHeight="10956" xr2:uid="{C0DCDE7E-FD22-412E-8C09-E69394502170}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>LastName</t>
   </si>
@@ -81,6 +81,36 @@
   </si>
   <si>
     <t>05/03/1977</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Мужской</t>
+  </si>
+  <si>
+    <t>Женский</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Калининградская область</t>
+  </si>
+  <si>
+    <t>Московская область</t>
+  </si>
+  <si>
+    <t>Санкт-Петербург</t>
+  </si>
+  <si>
+    <t>Гусев</t>
+  </si>
+  <si>
+    <t>Домодедово</t>
   </si>
 </sst>
 </file>
@@ -124,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -139,6 +169,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,21 +484,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715EC518-DB40-466B-8E2A-D97A4BF9CB0D}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -480,8 +514,17 @@
       <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -494,8 +537,17 @@
       <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -508,8 +560,17 @@
       <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -521,6 +582,15 @@
       </c>
       <c r="D4" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished RegistrationPage + Login Page + Requests Page
</commit_message>
<xml_diff>
--- a/test data/Merchants data.xlsx
+++ b/test data/Merchants data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Java\TS_Maven\test data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telesens\SKMaven\test data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB4F111-FF94-40A9-81D0-136E030FD975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB89F6C5-62BB-4B08-93F4-8B3E9FCF49E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C0DCDE7E-FD22-412E-8C09-E69394502170}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C0DCDE7E-FD22-412E-8C09-E69394502170}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>LastName</t>
   </si>
@@ -127,13 +127,82 @@
   </si>
   <si>
     <t>Республика Мордовия</t>
+  </si>
+  <si>
+    <t>Merchant Type</t>
+  </si>
+  <si>
+    <t>Специалист</t>
+  </si>
+  <si>
+    <t>Продавец</t>
+  </si>
+  <si>
+    <t>Физическое лицо</t>
+  </si>
+  <si>
+    <t>Юридическое лицо</t>
+  </si>
+  <si>
+    <t>ФЛП</t>
+  </si>
+  <si>
+    <t>ЗАО</t>
+  </si>
+  <si>
+    <t>Самозанятый</t>
+  </si>
+  <si>
+    <t>Название 1</t>
+  </si>
+  <si>
+    <t>Посуда топ</t>
+  </si>
+  <si>
+    <t>LE Or IP</t>
+  </si>
+  <si>
+    <t>Org Type</t>
+  </si>
+  <si>
+    <t>name RU</t>
+  </si>
+  <si>
+    <t>Какое-то</t>
+  </si>
+  <si>
+    <t>Mobilephone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>test1@test.test</t>
+  </si>
+  <si>
+    <t>test2@test.test</t>
+  </si>
+  <si>
+    <t>test3@test.test</t>
+  </si>
+  <si>
+    <t>Описание 1</t>
+  </si>
+  <si>
+    <t>Описание 2</t>
+  </si>
+  <si>
+    <t>Описание 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +220,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,10 +250,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -192,8 +270,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -506,25 +591,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715EC518-DB40-466B-8E2A-D97A4BF9CB0D}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" customWidth="1"/>
+    <col min="15" max="15" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -549,8 +641,29 @@
       <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -575,8 +688,29 @@
       <c r="H2" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="I2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="1">
+        <v>111111111</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -601,8 +735,29 @@
       <c r="H3" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="I3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="1">
+        <v>222333444</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -626,12 +781,38 @@
       </c>
       <c r="H4" s="5" t="s">
         <v>29</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="1">
+        <v>444555332</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{D09D9C43-629F-4489-9A69-F9BFA727FF89}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{626901EA-A166-45DB-9B49-445D0CA2E563}"/>
+    <hyperlink ref="N4" r:id="rId3" xr:uid="{44E1690B-A9B5-4EBE-8C56-41F0B1ACF456}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -643,9 +824,9 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -671,7 +852,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>

</xml_diff>